<commit_message>
Update Code Using DP
</commit_message>
<xml_diff>
--- a/D - Basic Algorithms 2/II. Dynamic Programming/dp_draft.xlsx
+++ b/D - Basic Algorithms 2/II. Dynamic Programming/dp_draft.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LCS" sheetId="1" r:id="rId1"/>
     <sheet name="Subset Sum" sheetId="2" r:id="rId2"/>
+    <sheet name="LPS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>a</t>
   </si>
@@ -82,6 +83,21 @@
   </si>
   <si>
     <t>DP = SubsetSum() || SubsetSum()</t>
+  </si>
+  <si>
+    <t>i/j</t>
+  </si>
+  <si>
+    <t>len</t>
+  </si>
+  <si>
+    <t>dp[I + 1][j - 1]</t>
+  </si>
+  <si>
+    <t>j = i + len - 1</t>
+  </si>
+  <si>
+    <t>I &lt;= n - len + 1</t>
   </si>
 </sst>
 </file>
@@ -130,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -145,6 +161,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,4 +878,542 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:J41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f>D23+C23-1</f>
+        <v>3</v>
+      </c>
+      <c r="G23" t="str">
+        <f>CONCATENATE(D23+1," ",E23-1)</f>
+        <v>2 2</v>
+      </c>
+      <c r="I23">
+        <f>7 - C23 +1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E27" si="0">D24+C24-1</f>
+        <v>4</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" ref="G24:G27" si="1">CONCATENATE(D24+1," ",E24-1)</f>
+        <v>3 3</v>
+      </c>
+      <c r="I24">
+        <f>7 - C24 +1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>4 4</v>
+      </c>
+      <c r="I25">
+        <f>7 - C25 +1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>5 5</v>
+      </c>
+      <c r="I26">
+        <f>7 - C26 +1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>6 6</v>
+      </c>
+      <c r="I27">
+        <f>7 - C27 +1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f>D29+C29-1</f>
+        <v>4</v>
+      </c>
+      <c r="G29" t="str">
+        <f>CONCATENATE(D29+1," ",E29-1)</f>
+        <v>2 3</v>
+      </c>
+      <c r="I29">
+        <f>7 - C29 +1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <f>D30+C30-1</f>
+        <v>5</v>
+      </c>
+      <c r="G30" t="str">
+        <f>CONCATENATE(D30+1," ",E30-1)</f>
+        <v>3 4</v>
+      </c>
+      <c r="I30">
+        <f>7 - C30 +1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <f>D31+C31-1</f>
+        <v>6</v>
+      </c>
+      <c r="G31" t="str">
+        <f>CONCATENATE(D31+1," ",E31-1)</f>
+        <v>4 5</v>
+      </c>
+      <c r="I31">
+        <f>7 - C31 +1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <f>D32+C32-1</f>
+        <v>7</v>
+      </c>
+      <c r="G32" t="str">
+        <f>CONCATENATE(D32+1," ",E32-1)</f>
+        <v>5 6</v>
+      </c>
+      <c r="I32">
+        <f>7 - C32 +1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E33:E41" si="2">D34+C34-1</f>
+        <v>5</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" ref="G33:G41" si="3">CONCATENATE(D34+1," ",E34-1)</f>
+        <v>2 4</v>
+      </c>
+      <c r="I34">
+        <f t="shared" ref="I33:I41" si="4">7 - C34 +1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="3"/>
+        <v>3 5</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="3"/>
+        <v>4 6</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="3"/>
+        <v>2 5</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="3"/>
+        <v>3 6</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="3"/>
+        <v>2 6</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>